<commit_message>
RED I2C pull-ups mark as DNP (BUS and UHF)
</commit_message>
<xml_diff>
--- a/BOM/OBC_FM_BOM.xlsx
+++ b/BOM/OBC_FM_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikas\Desktop\peaksat-repos\OBCBoard_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C1A4C-7F3D-43AC-8378-A7301CC8DA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D191E7E-42FC-4A61-97D3-F15621E6C1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBC_BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="239">
   <si>
     <t>Id</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>https://gr.mouser.com/ProductDetail/Panasonic/ERJ-2RKF1003X?qs=H7k1u0Mp9JQnXoBKdf15Qg%3D%3D</t>
-  </si>
-  <si>
-    <t>R130,R48,R47,R131,R9,R10,R20,R24,R14,R15</t>
   </si>
   <si>
     <t>1.5k</t>
@@ -760,6 +757,12 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Samtec/ESQ-126-14-G-D-LL?qs=3%252BjIH0OdpA%252BquPqGEkv%252Bag%3D%3D</t>
+  </si>
+  <si>
+    <t>R9, R10, R20, R24</t>
+  </si>
+  <si>
+    <t>R130,R48,R47,R131,R14,R15</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +859,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -870,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -928,6 +937,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -935,6 +957,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1144,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1002"/>
+  <dimension ref="A1:L1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1376,19 +1403,19 @@
     <row r="7" spans="1:12" s="18" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="14">
         <v>1</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1570,7 +1597,7 @@
     <row r="13" spans="1:12" s="18" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>40</v>
@@ -1582,7 +1609,7 @@
         <v>330</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="14"/>
@@ -1596,7 +1623,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>238</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
@@ -1605,10 +1632,10 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="G14" s="3">
         <v>0.01</v>
@@ -1627,48 +1654,34 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="69" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:12" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="1:12" ht="69" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="1">
-        <v>-55</v>
-      </c>
-      <c r="I15" s="1">
-        <v>155</v>
-      </c>
-      <c r="J15" s="1">
-        <v>50</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>13</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
@@ -1677,85 +1690,85 @@
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="H16" s="1">
         <v>-55</v>
       </c>
       <c r="I16" s="1">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="J16" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="1">
         <v>-55</v>
       </c>
       <c r="I17" s="1">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="J17" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="69" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1">
-        <v>6</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>120</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1">
         <v>-55</v>
@@ -1767,31 +1780,31 @@
         <v>25</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="1">
         <v>-55</v>
@@ -1800,21 +1813,19 @@
         <v>155</v>
       </c>
       <c r="J19" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>26</v>
@@ -1823,13 +1834,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" s="1">
         <v>-55</v>
@@ -1841,33 +1852,33 @@
         <v>10</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="69" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="1">
         <v>-55</v>
@@ -1876,106 +1887,108 @@
         <v>155</v>
       </c>
       <c r="J21" s="1">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="1">
         <v>-55</v>
       </c>
       <c r="I22" s="1">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="J22" s="1">
         <v>25</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H23" s="1">
         <v>-55</v>
       </c>
       <c r="I23" s="1">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="J23" s="1">
         <v>25</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="D24" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.01</v>
+        <v>72</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="H24" s="1">
         <v>-55</v>
@@ -1984,7 +1997,7 @@
         <v>155</v>
       </c>
       <c r="J24" s="1">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>29</v>
@@ -1993,46 +2006,46 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.01</v>
       </c>
       <c r="H25" s="1">
         <v>-55</v>
       </c>
       <c r="I25" s="1">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="J25" s="1">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -2041,34 +2054,34 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H26" s="1">
         <v>-55</v>
       </c>
       <c r="I26" s="1">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="J26" s="1">
         <v>25</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>26</v>
@@ -2077,13 +2090,13 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" s="1">
         <v>-55</v>
@@ -2095,16 +2108,16 @@
         <v>25</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>26</v>
@@ -2113,13 +2126,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H28" s="1">
         <v>-55</v>
@@ -2131,16 +2144,16 @@
         <v>25</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>26</v>
@@ -2149,13 +2162,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H29" s="1">
         <v>-55</v>
@@ -2167,31 +2180,31 @@
         <v>25</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.01</v>
+        <v>89</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="H30" s="1">
         <v>-55</v>
@@ -2200,106 +2213,106 @@
         <v>155</v>
       </c>
       <c r="J30" s="1">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>14</v>
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="1">
+        <v>-55</v>
+      </c>
+      <c r="I31" s="1">
+        <v>155</v>
+      </c>
+      <c r="J31" s="1">
+        <v>100</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="1">
-        <v>-55</v>
-      </c>
-      <c r="I32" s="1">
-        <v>155</v>
-      </c>
-      <c r="J32" s="1">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H33" s="1">
         <v>-55</v>
@@ -2311,60 +2324,64 @@
         <v>25</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="D34" s="1">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0.1</v>
+        <v>99</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="H34" s="1">
         <v>-55</v>
       </c>
       <c r="I34" s="1">
-        <v>125</v>
-      </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="J34" s="1">
+        <v>25</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G35" s="3">
         <v>0.1</v>
@@ -2381,22 +2398,22 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="1">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G36" s="3">
         <v>0.1</v>
@@ -2413,22 +2430,22 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="1">
-        <v>8</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>113</v>
+        <v>4</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G37" s="3">
         <v>0.1</v>
@@ -2439,33 +2456,31 @@
       <c r="I37" s="1">
         <v>125</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" s="1">
-        <v>4</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>116</v>
+        <v>8</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G38" s="3">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H38" s="1">
         <v>-55</v>
@@ -2473,31 +2488,33 @@
       <c r="I38" s="1">
         <v>125</v>
       </c>
-      <c r="J38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="G39" s="3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H39" s="1">
         <v>-55</v>
@@ -2511,22 +2528,22 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G40" s="3">
         <v>0.1</v>
@@ -2543,22 +2560,22 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G41" s="3">
         <v>0.1</v>
@@ -2575,22 +2592,22 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D42" s="1">
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G42" s="3">
         <v>0.1</v>
@@ -2607,53 +2624,57 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>-55</v>
+      </c>
+      <c r="I43" s="1">
+        <v>125</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D44" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2661,85 +2682,85 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" s="9" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
+    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" s="9" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
         <v>42</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B46" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D46" s="7">
+        <v>2</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="F46" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="D45" s="7">
-        <v>2</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>43</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="1">
-        <v>4</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D47" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -2749,25 +2770,25 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D48" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2777,25 +2798,25 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1">
         <v>4</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -2805,25 +2826,25 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2833,25 +2854,25 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="D51" s="1">
         <v>2</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>155</v>
+      <c r="E51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -2861,25 +2882,25 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="D52" s="1">
         <v>2</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>159</v>
+      <c r="E52" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -2889,25 +2910,25 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D53" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -2917,25 +2938,25 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D54" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -2945,25 +2966,25 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -2973,25 +2994,25 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -3001,25 +3022,25 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D57" s="1">
         <v>2</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -3029,25 +3050,25 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D58" s="1">
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3057,25 +3078,25 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D59" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -3085,25 +3106,25 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D60" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -3113,25 +3134,25 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D61" s="1">
         <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -3141,25 +3162,25 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D62" s="1">
         <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3169,25 +3190,25 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D63" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -3197,25 +3218,25 @@
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D64" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -3225,25 +3246,25 @@
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C65" s="1">
-        <v>5040500491</v>
+        <v>201</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="D65" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -3253,25 +3274,25 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C66" s="1">
-        <v>5037630691</v>
+        <v>5040500491</v>
       </c>
       <c r="D66" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -3281,25 +3302,25 @@
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="C67" s="1">
+        <v>5037630691</v>
       </c>
       <c r="D67" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -3307,81 +3328,81 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" s="18" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>64</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="1:12" s="18" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="14">
         <v>65</v>
       </c>
-      <c r="B68" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C68" s="19" t="s">
+      <c r="B69" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="14">
+        <v>2</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F69" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="D68" s="14">
-        <v>2</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-    </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>66</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
     </row>
     <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -3391,37 +3412,64 @@
     </row>
     <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>14</v>
+        <v>222</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>68</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+    </row>
     <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4352,6 +4400,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4360,61 +4409,61 @@
     <hyperlink ref="F11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F36" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="F37" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="F38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F39" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F43" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F44" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F45" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F46" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="F47" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F48" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="F49" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F50" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="F51" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="F52" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="F53" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F54" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="F55" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="F56" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="F57" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="F58" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="F59" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F60" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="F61" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="F62" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="F63" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="F64" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="F65" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="F66" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="F67" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="F68" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="F69" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="F70" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F24" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F30" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F34" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F36" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F38" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F39" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F40" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F41" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F42" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F43" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F44" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F45" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F46" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F47" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F48" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F49" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F50" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F51" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F52" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F53" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F54" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F55" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F56" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F57" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F58" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F59" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F60" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F61" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F62" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F63" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F64" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F65" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F66" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F68" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F69" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F70" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F71" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="F13" r:id="rId62" xr:uid="{32825C13-65E1-4588-921F-DEBF48D47F6D}"/>
     <hyperlink ref="F7" r:id="rId63" xr:uid="{CA127E7A-24AB-4C76-8920-40CDC22267B6}"/>
   </hyperlinks>

</xml_diff>